<commit_message>
Update DeliveryPlatform configuration and enhance delivery scheduling logic. Changed service addresses to use a specific hostname for local development. Added new product entries in stores CSV and adjusted truck capacities for improved delivery efficiency. Enhanced delivery reporting in schedule CSV with updated total distance and cost calculations, supporting partial deliveries in the scheduling logic.
</commit_message>
<xml_diff>
--- a/output/schedule_new.xlsx
+++ b/output/schedule_new.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="83">
   <si>
     <t>Маршрут</t>
   </si>
@@ -92,61 +92,157 @@
     <t>ROUTE_2</t>
   </si>
   <si>
+    <t>TRUCK_008</t>
+  </si>
+  <si>
+    <t>STORE_004</t>
+  </si>
+  <si>
+    <t>PROD_008</t>
+  </si>
+  <si>
+    <t>09:00</t>
+  </si>
+  <si>
+    <t>09:15</t>
+  </si>
+  <si>
+    <t>PROD_009</t>
+  </si>
+  <si>
+    <t>ROUTE_3</t>
+  </si>
+  <si>
     <t>TRUCK_007</t>
   </si>
   <si>
-    <t>STORE_004</t>
-  </si>
-  <si>
-    <t>PROD_008</t>
-  </si>
-  <si>
-    <t>09:00</t>
-  </si>
-  <si>
-    <t>09:15</t>
-  </si>
-  <si>
-    <t>PROD_009</t>
-  </si>
-  <si>
-    <t>ROUTE_3</t>
+    <t>STORE_010</t>
+  </si>
+  <si>
+    <t>PROD_003</t>
+  </si>
+  <si>
+    <t>10:16</t>
+  </si>
+  <si>
+    <t>PROD_007</t>
+  </si>
+  <si>
+    <t>ROUTE_4</t>
   </si>
   <si>
     <t>TRUCK_001</t>
   </si>
   <si>
+    <t>STORE_012</t>
+  </si>
+  <si>
+    <t>PROD_002</t>
+  </si>
+  <si>
+    <t>11:00</t>
+  </si>
+  <si>
+    <t>11:19</t>
+  </si>
+  <si>
+    <t>ROUTE_5</t>
+  </si>
+  <si>
+    <t>TRUCK_005</t>
+  </si>
+  <si>
+    <t>STORE_006</t>
+  </si>
+  <si>
+    <t>PROD_001</t>
+  </si>
+  <si>
+    <t>10:30</t>
+  </si>
+  <si>
+    <t>10:49</t>
+  </si>
+  <si>
+    <t>ROUTE_6</t>
+  </si>
+  <si>
+    <t>TRUCK_002</t>
+  </si>
+  <si>
+    <t>STORE_007</t>
+  </si>
+  <si>
+    <t>09:21</t>
+  </si>
+  <si>
+    <t>ROUTE_7</t>
+  </si>
+  <si>
+    <t>TRUCK_006</t>
+  </si>
+  <si>
+    <t>STORE_009</t>
+  </si>
+  <si>
+    <t>09:55</t>
+  </si>
+  <si>
+    <t>ROUTE_8</t>
+  </si>
+  <si>
+    <t>STORE_003</t>
+  </si>
+  <si>
+    <t>10:11</t>
+  </si>
+  <si>
+    <t>10:29</t>
+  </si>
+  <si>
+    <t>ROUTE_9</t>
+  </si>
+  <si>
     <t>STORE_005</t>
   </si>
   <si>
-    <t>PROD_002</t>
-  </si>
-  <si>
-    <t>11:00</t>
-  </si>
-  <si>
     <t>11:18</t>
   </si>
   <si>
     <t>PROD_010</t>
   </si>
   <si>
-    <t>ROUTE_4</t>
-  </si>
-  <si>
-    <t>TRUCK_005</t>
-  </si>
-  <si>
-    <t>STORE_010</t>
-  </si>
-  <si>
-    <t>PROD_003</t>
-  </si>
-  <si>
-    <t>10:16</t>
-  </si>
-  <si>
-    <t>PROD_007</t>
+    <t>ROUTE_10</t>
+  </si>
+  <si>
+    <t>STORE_011</t>
+  </si>
+  <si>
+    <t>10:27</t>
+  </si>
+  <si>
+    <t>10:51</t>
+  </si>
+  <si>
+    <t>ROUTE_11</t>
+  </si>
+  <si>
+    <t>STORE_001</t>
+  </si>
+  <si>
+    <t>11:30</t>
+  </si>
+  <si>
+    <t>11:55</t>
+  </si>
+  <si>
+    <t>ROUTE_12</t>
+  </si>
+  <si>
+    <t>STORE_008</t>
+  </si>
+  <si>
+    <t>11:33</t>
   </si>
   <si>
     <t>ИТОГИ</t>
@@ -249,13 +345,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.00390625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="10.57421875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.47265625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="24.77734375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="23.8046875" customWidth="true" bestFit="true"/>
@@ -571,10 +667,10 @@
         <v>34</v>
       </c>
       <c r="F7" t="n" s="3">
-        <v>5.0</v>
+        <v>28.0</v>
       </c>
       <c r="G7" t="n" s="3">
-        <v>45.0</v>
+        <v>22.0</v>
       </c>
       <c r="H7" t="s">
         <v>35</v>
@@ -583,22 +679,22 @@
         <v>8.0</v>
       </c>
       <c r="J7" t="n" s="3">
-        <v>2.4</v>
+        <v>3.2</v>
       </c>
       <c r="K7" t="n" s="3">
-        <v>45.28</v>
+        <v>35.61</v>
       </c>
       <c r="L7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" t="s">
         <v>36</v>
       </c>
-      <c r="M7" t="s">
-        <v>37</v>
-      </c>
       <c r="N7" t="n" s="3">
-        <v>90.55692569068708</v>
+        <v>71.21898762952972</v>
       </c>
       <c r="O7" t="n" s="4">
-        <v>950.8477197522143</v>
+        <v>712.1898762952972</v>
       </c>
     </row>
     <row r="8">
@@ -618,173 +714,1066 @@
         <v>34</v>
       </c>
       <c r="F8" t="n" s="3">
-        <v>5.0</v>
+        <v>28.0</v>
       </c>
       <c r="G8" t="n" s="3">
-        <v>45.0</v>
+        <v>22.0</v>
       </c>
       <c r="H8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I8" t="n" s="5">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="J8" t="n" s="3">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="K8" t="n" s="3">
-        <v>45.28</v>
+        <v>35.61</v>
       </c>
       <c r="L8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" t="s">
         <v>36</v>
       </c>
-      <c r="M8" t="s">
-        <v>37</v>
-      </c>
       <c r="N8" t="n" s="3">
-        <v>90.55692569068708</v>
+        <v>71.21898762952972</v>
       </c>
       <c r="O8" t="n" s="4">
-        <v>950.8477197522143</v>
+        <v>712.1898762952972</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
         <v>39</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
         <v>40</v>
       </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F9" t="n" s="3">
+        <v>42.0</v>
+      </c>
+      <c r="G9" t="n" s="3">
+        <v>18.0</v>
+      </c>
+      <c r="H9" t="s">
         <v>41</v>
       </c>
-      <c r="F9" t="n" s="3">
-        <v>28.0</v>
-      </c>
-      <c r="G9" t="n" s="3">
-        <v>22.0</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="I9" t="n" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="J9" t="n" s="3">
+        <v>2.6999999999999997</v>
+      </c>
+      <c r="K9" t="n" s="3">
+        <v>45.69</v>
+      </c>
+      <c r="L9" t="s">
         <v>42</v>
-      </c>
-      <c r="I9" t="n" s="5">
-        <v>8.0</v>
-      </c>
-      <c r="J9" t="n" s="3">
-        <v>3.2</v>
-      </c>
-      <c r="K9" t="n" s="3">
-        <v>35.61</v>
-      </c>
-      <c r="L9" t="s">
-        <v>22</v>
       </c>
       <c r="M9" t="s">
         <v>43</v>
       </c>
       <c r="N9" t="n" s="3">
-        <v>71.21898762952972</v>
+        <v>91.38463863518345</v>
       </c>
       <c r="O9" t="n" s="4">
-        <v>783.408863924827</v>
+        <v>959.5387056694262</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
         <v>39</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
         <v>40</v>
       </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" t="s">
-        <v>41</v>
-      </c>
       <c r="F10" t="n" s="3">
-        <v>28.0</v>
+        <v>42.0</v>
       </c>
       <c r="G10" t="n" s="3">
-        <v>22.0</v>
+        <v>18.0</v>
       </c>
       <c r="H10" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="I10" t="n" s="5">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="J10" t="n" s="3">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="K10" t="n" s="3">
-        <v>35.61</v>
+        <v>45.69</v>
       </c>
       <c r="L10" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="M10" t="s">
         <v>43</v>
       </c>
       <c r="N10" t="n" s="3">
-        <v>71.21898762952972</v>
+        <v>91.38463863518345</v>
       </c>
       <c r="O10" t="n" s="4">
-        <v>783.408863924827</v>
+        <v>959.5387056694262</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" t="n" s="3">
+        <v>40.0</v>
+      </c>
+      <c r="G11" t="n" s="3">
+        <v>25.0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" t="n" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="J11" t="n" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="K11" t="n" s="3">
+        <v>47.17</v>
+      </c>
+      <c r="L11" t="s">
+        <v>48</v>
+      </c>
+      <c r="M11" t="s">
+        <v>49</v>
+      </c>
+      <c r="N11" t="n" s="3">
+        <v>94.33990566028302</v>
+      </c>
+      <c r="O11" t="n" s="4">
+        <v>1037.7389622631133</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="n" s="3">
+        <v>40.0</v>
+      </c>
+      <c r="G12" t="n" s="3">
+        <v>25.0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" t="n" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="J12" t="n" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="K12" t="n" s="3">
+        <v>47.17</v>
+      </c>
+      <c r="L12" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N12" t="n" s="3">
+        <v>94.33990566028302</v>
+      </c>
+      <c r="O12" t="n" s="4">
+        <v>1037.7389622631133</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s" s="1">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
         <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="n" s="3">
+        <v>40.0</v>
+      </c>
+      <c r="G13" t="n" s="3">
+        <v>25.0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" t="n" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="J13" t="n" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="K13" t="n" s="3">
+        <v>47.17</v>
+      </c>
+      <c r="L13" t="s">
+        <v>48</v>
+      </c>
+      <c r="M13" t="s">
+        <v>49</v>
+      </c>
+      <c r="N13" t="n" s="3">
+        <v>94.33990566028302</v>
+      </c>
+      <c r="O13" t="n" s="4">
+        <v>1037.7389622631133</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" t="n" s="3">
-        <v>311.0403162571138</v>
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" t="n" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="G14" t="n" s="3">
+        <v>30.0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" t="n" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="J14" t="n" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="K14" t="n" s="3">
+        <v>36.06</v>
+      </c>
+      <c r="L14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M14" t="s">
+        <v>53</v>
+      </c>
+      <c r="N14" t="n" s="3">
+        <v>72.1155127546399</v>
+      </c>
+      <c r="O14" t="n" s="4">
+        <v>865.3861530556787</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" t="n" s="4">
-        <v>3209.6962877789683</v>
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" t="n" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="G15" t="n" s="3">
+        <v>30.0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" t="n" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="J15" t="n" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="K15" t="n" s="3">
+        <v>36.06</v>
+      </c>
+      <c r="L15" t="s">
+        <v>29</v>
+      </c>
+      <c r="M15" t="s">
+        <v>53</v>
+      </c>
+      <c r="N15" t="n" s="3">
+        <v>72.1155127546399</v>
+      </c>
+      <c r="O15" t="n" s="4">
+        <v>865.3861530556787</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" t="n" s="5">
-        <v>9.0</v>
+        <v>54</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" t="n" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="G16" t="n" s="3">
+        <v>28.0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" t="n" s="5">
+        <v>15.0</v>
+      </c>
+      <c r="J16" t="n" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="K16" t="n" s="3">
+        <v>30.46</v>
+      </c>
+      <c r="L16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M16" t="s">
+        <v>57</v>
+      </c>
+      <c r="N16" t="n" s="3">
+        <v>60.923092423455635</v>
+      </c>
+      <c r="O16" t="n" s="4">
+        <v>792.0002015049232</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" t="n" s="3">
-        <v>30.15</v>
+        <v>54</v>
+      </c>
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" t="n" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="G17" t="n" s="3">
+        <v>28.0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" t="n" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="J17" t="n" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="K17" t="n" s="3">
+        <v>30.46</v>
+      </c>
+      <c r="L17" t="s">
+        <v>21</v>
+      </c>
+      <c r="M17" t="s">
+        <v>57</v>
+      </c>
+      <c r="N17" t="n" s="3">
+        <v>60.923092423455635</v>
+      </c>
+      <c r="O17" t="n" s="4">
+        <v>792.0002015049232</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" t="n" s="5">
-        <v>4.0</v>
+        <v>58</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" t="n" s="3">
+        <v>15.0</v>
+      </c>
+      <c r="G18" t="n" s="3">
+        <v>40.0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>47</v>
+      </c>
+      <c r="I18" t="n" s="5">
+        <v>12.0</v>
+      </c>
+      <c r="J18" t="n" s="3">
+        <v>6.0</v>
+      </c>
+      <c r="K18" t="n" s="3">
+        <v>42.72</v>
+      </c>
+      <c r="L18" t="s">
+        <v>60</v>
+      </c>
+      <c r="M18" t="s">
+        <v>61</v>
+      </c>
+      <c r="N18" t="n" s="3">
+        <v>85.44001872658765</v>
+      </c>
+      <c r="O18" t="n" s="4">
+        <v>837.3121835205591</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" t="n" s="3">
+        <v>15.0</v>
+      </c>
+      <c r="G19" t="n" s="3">
+        <v>40.0</v>
+      </c>
+      <c r="H19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" t="n" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="J19" t="n" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="K19" t="n" s="3">
+        <v>42.72</v>
+      </c>
+      <c r="L19" t="s">
+        <v>60</v>
+      </c>
+      <c r="M19" t="s">
+        <v>61</v>
+      </c>
+      <c r="N19" t="n" s="3">
+        <v>85.44001872658765</v>
+      </c>
+      <c r="O19" t="n" s="4">
+        <v>837.3121835205591</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" t="n" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="G20" t="n" s="3">
+        <v>45.0</v>
+      </c>
+      <c r="H20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20" t="n" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="J20" t="n" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="K20" t="n" s="3">
+        <v>45.28</v>
+      </c>
+      <c r="L20" t="s">
+        <v>42</v>
+      </c>
+      <c r="M20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N20" t="n" s="3">
+        <v>90.55692569068708</v>
+      </c>
+      <c r="O20" t="n" s="4">
+        <v>905.5692569068708</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" t="n" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="G21" t="n" s="3">
+        <v>45.0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>65</v>
+      </c>
+      <c r="I21" t="n" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="J21" t="n" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="K21" t="n" s="3">
+        <v>45.28</v>
+      </c>
+      <c r="L21" t="s">
+        <v>42</v>
+      </c>
+      <c r="M21" t="s">
+        <v>64</v>
+      </c>
+      <c r="N21" t="n" s="3">
+        <v>90.55692569068708</v>
+      </c>
+      <c r="O21" t="n" s="4">
+        <v>905.5692569068708</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" t="n" s="3">
+        <v>18.0</v>
+      </c>
+      <c r="G22" t="n" s="3">
+        <v>38.0</v>
+      </c>
+      <c r="H22" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" t="n" s="5">
+        <v>12.0</v>
+      </c>
+      <c r="J22" t="n" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="K22" t="n" s="3">
+        <v>42.05</v>
+      </c>
+      <c r="L22" t="s">
+        <v>68</v>
+      </c>
+      <c r="M22" t="s">
+        <v>69</v>
+      </c>
+      <c r="N22" t="n" s="3">
+        <v>84.09759208325727</v>
+      </c>
+      <c r="O22" t="n" s="4">
+        <v>840.9759208325727</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23" t="n" s="3">
+        <v>18.0</v>
+      </c>
+      <c r="G23" t="n" s="3">
+        <v>38.0</v>
+      </c>
+      <c r="H23" t="s">
+        <v>65</v>
+      </c>
+      <c r="I23" t="n" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="J23" t="n" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="K23" t="n" s="3">
+        <v>42.05</v>
+      </c>
+      <c r="L23" t="s">
+        <v>68</v>
+      </c>
+      <c r="M23" t="s">
+        <v>69</v>
+      </c>
+      <c r="N23" t="n" s="3">
+        <v>84.09759208325727</v>
+      </c>
+      <c r="O23" t="n" s="4">
+        <v>840.9759208325727</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F24" t="n" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="G24" t="n" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="H24" t="s">
+        <v>47</v>
+      </c>
+      <c r="I24" t="n" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="J24" t="n" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="K24" t="n" s="3">
+        <v>22.36</v>
+      </c>
+      <c r="L24" t="s">
+        <v>72</v>
+      </c>
+      <c r="M24" t="s">
+        <v>73</v>
+      </c>
+      <c r="N24" t="n" s="3">
+        <v>44.7206797749979</v>
+      </c>
+      <c r="O24" t="n" s="4">
+        <v>469.5671376374779</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" t="n" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="G25" t="n" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>41</v>
+      </c>
+      <c r="I25" t="n" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="J25" t="n" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="K25" t="n" s="3">
+        <v>22.36</v>
+      </c>
+      <c r="L25" t="s">
+        <v>72</v>
+      </c>
+      <c r="M25" t="s">
+        <v>73</v>
+      </c>
+      <c r="N25" t="n" s="3">
+        <v>44.7206797749979</v>
+      </c>
+      <c r="O25" t="n" s="4">
+        <v>469.5671376374779</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" t="s">
+        <v>71</v>
+      </c>
+      <c r="F26" t="n" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="G26" t="n" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="H26" t="s">
+        <v>35</v>
+      </c>
+      <c r="I26" t="n" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="J26" t="n" s="3">
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="K26" t="n" s="3">
+        <v>22.36</v>
+      </c>
+      <c r="L26" t="s">
+        <v>72</v>
+      </c>
+      <c r="M26" t="s">
+        <v>73</v>
+      </c>
+      <c r="N26" t="n" s="3">
+        <v>44.7206797749979</v>
+      </c>
+      <c r="O26" t="n" s="4">
+        <v>469.5671376374779</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" t="n" s="3">
+        <v>10.0</v>
+      </c>
+      <c r="G27" t="n" s="3">
+        <v>20.0</v>
+      </c>
+      <c r="H27" t="s">
+        <v>28</v>
+      </c>
+      <c r="I27" t="n" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="J27" t="n" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="K27" t="n" s="3">
+        <v>22.36</v>
+      </c>
+      <c r="L27" t="s">
+        <v>72</v>
+      </c>
+      <c r="M27" t="s">
+        <v>73</v>
+      </c>
+      <c r="N27" t="n" s="3">
+        <v>44.7206797749979</v>
+      </c>
+      <c r="O27" t="n" s="4">
+        <v>469.5671376374779</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" t="s">
+        <v>75</v>
+      </c>
+      <c r="F28" t="n" s="3">
+        <v>35.0</v>
+      </c>
+      <c r="G28" t="n" s="3">
+        <v>15.0</v>
+      </c>
+      <c r="H28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I28" t="n" s="5">
+        <v>20.0</v>
+      </c>
+      <c r="J28" t="n" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="K28" t="n" s="3">
+        <v>38.08</v>
+      </c>
+      <c r="L28" t="s">
+        <v>42</v>
+      </c>
+      <c r="M28" t="s">
+        <v>76</v>
+      </c>
+      <c r="N28" t="n" s="3">
+        <v>76.15886552931954</v>
+      </c>
+      <c r="O28" t="n" s="4">
+        <v>837.747520822515</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" t="n" s="3">
+        <v>35.0</v>
+      </c>
+      <c r="G29" t="n" s="3">
+        <v>15.0</v>
+      </c>
+      <c r="H29" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" t="n" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="J29" t="n" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="K29" t="n" s="3">
+        <v>38.08</v>
+      </c>
+      <c r="L29" t="s">
+        <v>42</v>
+      </c>
+      <c r="M29" t="s">
+        <v>76</v>
+      </c>
+      <c r="N29" t="n" s="3">
+        <v>76.15886552931954</v>
+      </c>
+      <c r="O29" t="n" s="4">
+        <v>837.747520822515</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" t="n" s="3">
+        <v>920.2206218448381</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" t="n" s="4">
+        <v>9733.465622610362</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" t="n" s="5">
+        <v>28.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" t="n" s="3">
+        <v>100.85000000000002</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" t="n" s="5">
+        <v>12.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>